<commit_message>
update employee import template file (#570)
</commit_message>
<xml_diff>
--- a/apps/hrm/fixtures/import_templates/employee_template.xlsx
+++ b/apps/hrm/fixtures/import_templates/employee_template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manh/Downloads/projects/maivietland/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25964FDF-EBD8-BC42-AFB0-9C7B7353AD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F705ACA5-E792-3044-85C8-BB5AA9DD7DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{BA4144E9-4D9F-3B44-AF74-835FE8E52AAC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet điền thông tin nhân viên" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet lưu thông tin mẫu" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1453,7 +1454,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="420">
   <si>
     <t>STT</t>
   </si>
@@ -2603,13 +2604,124 @@
   </si>
   <si>
     <t>Số CMND/CCCD</t>
+  </si>
+  <si>
+    <t>Phòng ban</t>
+  </si>
+  <si>
+    <t>Loại hợp đồng</t>
+  </si>
+  <si>
+    <t>Hôn nhân</t>
+  </si>
+  <si>
+    <t>Lý do nghỉ việc</t>
+  </si>
+  <si>
+    <t>Chi nhánh 1</t>
+  </si>
+  <si>
+    <t>Khối 1</t>
+  </si>
+  <si>
+    <t>Phòng ban 1</t>
+  </si>
+  <si>
+    <t>Chức vụ 1</t>
+  </si>
+  <si>
+    <t>Đang làm việc (W)</t>
+  </si>
+  <si>
+    <t>Danh sách Quốc tịch trong hệ thống</t>
+  </si>
+  <si>
+    <t>Thỏa thuận chấm dứt Hợp đồng lao động trước thời hạn</t>
+  </si>
+  <si>
+    <t>Chi nhánh 2</t>
+  </si>
+  <si>
+    <t>Khối 2</t>
+  </si>
+  <si>
+    <t>Phòng ban 2</t>
+  </si>
+  <si>
+    <t>Chức vụ 2</t>
+  </si>
+  <si>
+    <t>Đã nghỉ việc (C)</t>
+  </si>
+  <si>
+    <t>Thử việc không đạt</t>
+  </si>
+  <si>
+    <t>Chi nhánh 3</t>
+  </si>
+  <si>
+    <t>Khối 3</t>
+  </si>
+  <si>
+    <t>Chức vụ 3</t>
+  </si>
+  <si>
+    <t>Nghỉ không lương</t>
+  </si>
+  <si>
+    <t>Ly hôn</t>
+  </si>
+  <si>
+    <t>Bỏ việc</t>
+  </si>
+  <si>
+    <t>Chi nhánh 4</t>
+  </si>
+  <si>
+    <t>Nghỉ thai sản</t>
+  </si>
+  <si>
+    <t>Sa thải do kỷ luật</t>
+  </si>
+  <si>
+    <t>Học việc</t>
+  </si>
+  <si>
+    <t>Thanh lọc</t>
+  </si>
+  <si>
+    <t>Thực tập sinh</t>
+  </si>
+  <si>
+    <t>Thành tích kém trong công việc</t>
+  </si>
+  <si>
+    <t>Thử việc loại 1</t>
+  </si>
+  <si>
+    <t>Hết hợp đồng</t>
+  </si>
+  <si>
+    <t>Nguyện vọng theo đơn - Không đảm bảo sức khỏe</t>
+  </si>
+  <si>
+    <t>Nguyện vọng theo đơn - Bận việc cá nhân</t>
+  </si>
+  <si>
+    <t>Nguyện vọng theo đơn - Thay đổi định hướng công việc</t>
+  </si>
+  <si>
+    <t>Nguyện vọng theo đơn - Khác</t>
+  </si>
+  <si>
+    <t>Khác</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2698,6 +2810,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2919,7 +3050,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3010,9 +3141,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3330,13 +3461,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5551D2-3CFD-DE41-A92F-38D9A084B00E}">
   <dimension ref="A1:AL27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:38" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -3561,7 +3692,9 @@
       <c r="H4" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="21"/>
+      <c r="I4" s="21" t="s">
+        <v>408</v>
+      </c>
       <c r="J4" s="22"/>
       <c r="K4" s="20" t="s">
         <v>42</v>
@@ -3663,7 +3796,9 @@
       <c r="H5" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="21" t="s">
+        <v>410</v>
+      </c>
       <c r="J5" s="22"/>
       <c r="K5" s="20" t="s">
         <v>67</v>
@@ -3767,7 +3902,9 @@
       <c r="H6" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="I6" s="21"/>
+      <c r="I6" s="21" t="s">
+        <v>414</v>
+      </c>
       <c r="J6" s="22"/>
       <c r="K6" s="20" t="s">
         <v>67</v>
@@ -3871,7 +4008,9 @@
       <c r="H7" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="I7" s="21"/>
+      <c r="I7" s="21" t="s">
+        <v>416</v>
+      </c>
       <c r="J7" s="22"/>
       <c r="K7" s="20" t="s">
         <v>67</v>
@@ -5925,5 +6064,302 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BBD31E9-DAAC-BE46-94C9-C35661D2F9BF}">
+          <x14:formula1>
+            <xm:f>'Sheet lưu thông tin mẫu'!$J$2:$J$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>I4:I27</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2550696C-3134-5447-91E6-8AE35803193B}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>384</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>389</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>390</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>391</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>395</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>397</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="33" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>401</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>402</v>
+      </c>
+      <c r="F4" s="34"/>
+      <c r="G4" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>404</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
+        <v>406</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="H5" s="34"/>
+      <c r="J5" s="33" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="33" t="s">
+        <v>409</v>
+      </c>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="J6" s="33" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="33" t="s">
+        <v>411</v>
+      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="33" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="33" t="s">
+        <v>413</v>
+      </c>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="33" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="33" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="33" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="33" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="33" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="33" t="s">
+        <v>419</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>